<commit_message>
Added conditional highlighting. Also various tweaks
</commit_message>
<xml_diff>
--- a/py_runner.xlsx
+++ b/py_runner.xlsx
@@ -9,6 +9,7 @@
   </bookViews>
   <sheets>
     <sheet name="Activities" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Info" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="62">
   <si>
     <t xml:space="preserve">Activity Run</t>
   </si>
@@ -28,16 +29,37 @@
     <t xml:space="preserve">Spreadsheet used by spreadsheet_py_runner.py</t>
   </si>
   <si>
+    <t xml:space="preserve">Optional condition applied to result</t>
+  </si>
+  <si>
     <t xml:space="preserve">Start Row:</t>
   </si>
   <si>
+    <t xml:space="preserve">Causes background colour to change</t>
+  </si>
+  <si>
     <t xml:space="preserve">End Row:</t>
   </si>
   <si>
-    <t xml:space="preserve">Action definitions in actions.py</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Args read as csv strings</t>
+    <t xml:space="preserve">Action values are the names of functions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arguments for the function</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Can use r or result to stand for result</t>
+  </si>
+  <si>
+    <t xml:space="preserve">present in actions.py</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Read as csv strings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Python, not Excel formula.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Result of check with optional colour highlighting. Colour key on Info tab.</t>
   </si>
   <si>
     <t xml:space="preserve">Skip</t>
@@ -52,6 +74,9 @@
     <t xml:space="preserve">Args</t>
   </si>
   <si>
+    <t xml:space="preserve">Condition</t>
+  </si>
+  <si>
     <t xml:space="preserve">Result</t>
   </si>
   <si>
@@ -73,12 +98,24 @@
     <t xml:space="preserve">1,2</t>
   </si>
   <si>
+    <t xml:space="preserve">result  == 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add two numbers – incorrect condition </t>
+  </si>
+  <si>
+    <t xml:space="preserve">r  == 4</t>
+  </si>
+  <si>
     <t xml:space="preserve">Generate Fibonacci series – arg is number of items after 1,2</t>
   </si>
   <si>
     <t xml:space="preserve">fibonacci</t>
   </si>
   <si>
+    <t xml:space="preserve">invalid thing makes purple!</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ping website – note result may not display well unless cell clicked</t>
   </si>
   <si>
@@ -88,25 +125,10 @@
     <t xml:space="preserve">www.bbc.co.uk</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF5D5D00"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Ping another website - </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF5D5D00"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">note result may not display well unless cell clicked</t>
-    </r>
+    <t xml:space="preserve">'0% packet loss' in result</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ping another website - note result may not display well unless cell clicked</t>
   </si>
   <si>
     <t xml:space="preserve">www.google.com</t>
@@ -121,6 +143,9 @@
     <t xml:space="preserve">https://portal.legalservices.gov.uk</t>
   </si>
   <si>
+    <t xml:space="preserve">result == 200</t>
+  </si>
+  <si>
     <t xml:space="preserve">Extract headings from site using Webdriver</t>
   </si>
   <si>
@@ -128,6 +153,60 @@
   </si>
   <si>
     <t xml:space="preserve">https://www.theregister.co.uk/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Two rows  below share data using share dictionary in action.py</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reads contents of text file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">read_file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">README.md,readme_data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Counts number of * characters within the file from above</t>
+  </si>
+  <si>
+    <t xml:space="preserve">count_occurs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*,readme_data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Result Colour Key</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Orange</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Execution failed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Green</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Execution completed and condition gave “pass” result</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Read</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Execution completed and condition gave “fail” result</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Purple</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Execution completed but evaluation of condition failed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Execution completed. No conditional highlighting applied.</t>
   </si>
 </sst>
 </file>
@@ -137,7 +216,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -177,6 +256,14 @@
       <charset val="1"/>
     </font>
     <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <b val="true"/>
       <sz val="11"/>
       <color rgb="FF0000DC"/>
@@ -192,9 +279,8 @@
       <charset val="1"/>
     </font>
     <font>
-      <i val="true"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -207,13 +293,15 @@
       <charset val="1"/>
     </font>
     <font>
+      <b val="true"/>
       <sz val="10"/>
       <color rgb="FF5D5D00"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -244,6 +332,30 @@
         <bgColor rgb="FFE0EFD4"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF8000"/>
+        <bgColor rgb="FFFF6600"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB2FF66"/>
+        <bgColor rgb="FFE0EFD4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF3333"/>
+        <bgColor rgb="FFFF6600"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC00CC"/>
+        <bgColor rgb="FFFF00FF"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
@@ -286,7 +398,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -299,15 +411,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -327,12 +451,40 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -348,11 +500,11 @@
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFE8E8E8"/>
-      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FFFF3333"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000DC"/>
       <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFCC00CC"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
       <rgbColor rgb="FF008000"/>
@@ -361,7 +513,7 @@
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFC0C0C0"/>
-      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF7F7F7F"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFFFFBCC"/>
@@ -381,7 +533,7 @@
       <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FFE0EFD4"/>
-      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FFB2FF66"/>
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
@@ -390,7 +542,7 @@
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF8000"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
@@ -412,22 +564,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:G19"/>
+  <dimension ref="B1:H20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="50.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="30.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="30.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="31.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="60.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="22.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="28.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="55.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="22.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -439,201 +592,282 @@
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="F2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="4" t="n">
+      <c r="B3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="6" t="n">
         <v>7</v>
       </c>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="8"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="4" t="n">
+      <c r="B4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="6" t="n">
+        <v>17</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="8"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="9" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D5" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="7" t="s">
+      <c r="C6" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="12"/>
+      <c r="C7" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="12"/>
+      <c r="C8" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="12"/>
+      <c r="C9" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="12"/>
+      <c r="C10" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="14" t="n">
         <v>8</v>
       </c>
-      <c r="E6" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="9"/>
-      <c r="C7" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="9"/>
-      <c r="C8" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="9"/>
-      <c r="C9" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" s="11" t="n">
-        <v>8</v>
-      </c>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="9"/>
-      <c r="C10" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
+      <c r="F10" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="9"/>
-      <c r="C11" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="9"/>
-      <c r="C12" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="9"/>
-      <c r="C13" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="9"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="9"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="9"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="9"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="9"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="9"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="12"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E10" r:id="rId1" display="www.bbc.co.uk"/>
-    <hyperlink ref="E11" r:id="rId2" display="www.google.com"/>
-    <hyperlink ref="E12" r:id="rId3" display="https://portal.legalservices.gov.uk"/>
-    <hyperlink ref="E13" r:id="rId4" display="https://www.theregister.co.uk/"/>
+    <hyperlink ref="E11" r:id="rId1" display="www.bbc.co.uk"/>
+    <hyperlink ref="E12" r:id="rId2" display="www.google.com"/>
+    <hyperlink ref="E13" r:id="rId3" display="https://portal.legalservices.gov.uk"/>
+    <hyperlink ref="E14" r:id="rId4" display="https://www.theregister.co.uk/"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
@@ -643,4 +877,76 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.67"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>